<commit_message>
Finished homeworks 1 and 2
</commit_message>
<xml_diff>
--- a/d_datos_orig_pena_llanos.xlsx
+++ b/d_datos_orig_pena_llanos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angie.llanos\Documents\Modelo\CredibilityModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C11168A-F464-4800-A557-1596BFD9F557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD949789-B998-41D3-8953-B91AA63A1A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="265">
   <si>
     <t>index</t>
   </si>
@@ -766,158 +766,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF3C4043"/>
-        <rFont val="Inherit"/>
-      </rPr>
-      <t xml:space="preserve">Company Name: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF3C4043"/>
-        <rFont val="Inherit"/>
-      </rPr>
-      <t>Nombre de la compañía de seguros de automóviles (String)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF3C4043"/>
-        <rFont val="Inherit"/>
-      </rPr>
-      <t>Ratio:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF3C4043"/>
-        <rFont val="Inherit"/>
-      </rPr>
-      <t xml:space="preserve"> Relación entre las reclamaciones estimadas y el total de reclamaciones (Float)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF3C4043"/>
-        <rFont val="Inherit"/>
-      </rPr>
-      <t xml:space="preserve">Premiums Written (in Millions): </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF3C4043"/>
-        <rFont val="Inherit"/>
-      </rPr>
-      <t>Primas totales emitidas en millones de dólares (Float)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF3C4043"/>
-        <rFont val="Inherit"/>
-      </rPr>
-      <t>Rank:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF3C4043"/>
-        <rFont val="Inherit"/>
-      </rPr>
-      <t xml:space="preserve"> Clasificación de la empresa en función de la tasa de reclamaciones (Integer)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF3C4043"/>
-        <rFont val="Inherit"/>
-      </rPr>
-      <t>Upheld Complaints:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF3C4043"/>
-        <rFont val="Inherit"/>
-      </rPr>
-      <t xml:space="preserve"> Número de reclamaciones confirmadas por el Departamento de Servicios Financieros (Integer)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF3C4043"/>
-        <rFont val="Inherit"/>
-      </rPr>
-      <t>Question of Fact Complaints:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF3C4043"/>
-        <rFont val="Inherit"/>
-      </rPr>
-      <t xml:space="preserve"> Número de reclamaciones que requieren una investigación más profunda (Integer)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF3C4043"/>
-        <rFont val="Inherit"/>
-      </rPr>
-      <t xml:space="preserve">Not Upheld Complaints: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF3C4043"/>
-        <rFont val="Inherit"/>
-      </rPr>
-      <t>Número de reclamaciones no aceptadas por el Departamento de Servicios Financieros (Integer)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF3C4043"/>
-        <rFont val="Inherit"/>
-      </rPr>
-      <t xml:space="preserve">Total Complaints: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF3C4043"/>
-        <rFont val="Inherit"/>
-      </rPr>
-      <t>Número total de reclamaciones (Integer)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">2009 - 2016.  Para no ver los datos como una serie de tiempo se utilizarán únicamente los datos relativos al año más actual, </t>
     </r>
     <r>
@@ -943,25 +791,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF3C4043"/>
-        <rFont val="Inherit"/>
-      </rPr>
-      <t>Filing Year:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF3C4043"/>
-        <rFont val="Inherit"/>
-      </rPr>
-      <t xml:space="preserve"> Año en el que se presentaron los datos de la reclamación (Integer)</t>
-    </r>
-  </si>
-  <si>
     <t>Compañías de seguros de automóviles en el estado de Nueva York</t>
   </si>
   <si>
@@ -983,7 +812,45 @@
         <color rgb="FF3C4043"/>
         <rFont val="Inherit"/>
       </rPr>
-      <t>(String)</t>
+      <t>(String) Como no es una variable numérica sino cadena de caracteres, no puede tomar el valor 0, pues signifcaría que no hay aseguradora en esa línea de datos, lo cual es absurdo para una línea de datos existente.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t xml:space="preserve">NAIC: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>Código de seis dígitos asignado por la National Association of Insurance Commissioners.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t xml:space="preserve">Company Name: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>Nombre de la compañía de seguros de automóviles.</t>
     </r>
   </si>
   <si>
@@ -1002,7 +869,7 @@
         <color rgb="FF3C4043"/>
         <rFont val="Inherit"/>
       </rPr>
-      <t xml:space="preserve"> (Float)</t>
+      <t xml:space="preserve"> Relación entre las reclamaciones estimadas y el total de reclamaciones.</t>
     </r>
   </si>
   <si>
@@ -1013,7 +880,7 @@
         <color rgb="FF3C4043"/>
         <rFont val="Inherit"/>
       </rPr>
-      <t xml:space="preserve">NAIC: </t>
+      <t>Upheld Complaints:</t>
     </r>
     <r>
       <rPr>
@@ -1021,7 +888,7 @@
         <color rgb="FF3C4043"/>
         <rFont val="Inherit"/>
       </rPr>
-      <t>Código de seis dígitos asignado por la National Association of Insurance Commissioners (Integer)</t>
+      <t xml:space="preserve"> Número de reclamaciones confirmadas por el Departamento de Servicios Financieros.</t>
     </r>
   </si>
   <si>
@@ -1032,7 +899,7 @@
         <color rgb="FF3C4043"/>
         <rFont val="Inherit"/>
       </rPr>
-      <t xml:space="preserve">NAIC: </t>
+      <t>Question of Fact Complaints:</t>
     </r>
     <r>
       <rPr>
@@ -1040,10 +907,279 @@
         <color rgb="FF3C4043"/>
         <rFont val="Inherit"/>
       </rPr>
-      <t>(Integer) El soporte de la variable en este conjunto de datos está en el intervalo [10000, 44000]. Esta variable no puede tomar el valor de 0 en todos sus dígitos; el 0 eventualmente se usa como prefijo, solo cuando:
+      <t xml:space="preserve"> Número de reclamaciones que requieren una investigación más profunda.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t xml:space="preserve">Not Upheld Complaints: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>Número de reclamaciones no aceptadas por el Departamento de Servicios Financieros.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t xml:space="preserve">Total Complaints: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>Número total de reclamaciones.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t xml:space="preserve">Premiums Written (in Millions): </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>Primas totales emitidas en millones de dólares.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>Rank:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t xml:space="preserve"> Clasificación de la empresa en función de la tasa de reclamaciones.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>Filing Year:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t xml:space="preserve"> Año en el que se presentaron los datos de la reclamación.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>Ratio:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t xml:space="preserve"> (Float) El soporte de la variable pertenece al intervalo [0, 1400). Es cero, cuando las reclamaciones estimadas son cero, es menor a 1 cuando las reclamaciones estimadas son menores al total de reclamaciones y mayor a 1, cuando son mayores.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>NAIC:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer) El soporte de la variable pertenece al intervalo [10000, 44000]. Esta variable no puede tomar el valor de 0 en todos sus dígitos; el 0 eventualmente se usa como prefijo, solo cuando:
 * La compañía de seguros sea una entidad extranjera que no está autorizada para hacer negocios en los Estados Unidos, pero que tiene operaciones en el país a través de una sucursal o una subsidiaria. En este caso, el código seguido del 0 es el código asignado por el país de origen de la compañía.
 * La compañía de seguros es una entidad recién formada que aún no ha recibido un código NAIC. En este caso, el código seguido del 0 es el número de identificación fiscal (TIN) de la compañía hasta que se le asigne un código NAIC definitivo.
 * La compañía de seguros es una entidad que ha dejado de operar o que ha sido liquidada. En este caso, el código seguido del 0  es el último código NAIC que tuvo la compañía antes de cesar sus actividades.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>Upheld Complaints:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer) El soporte de la variable pertenece al conjunto {0,1,2,…,265}. El valor de cero significa que no hubieron reclamaciones confirmadas por el departamento de servicios financieros.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>Question of Fact Complaints:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer) El soporte de la variable pertenece al conjunto {0,1,2,…,698}. El valor de cero significa que no hubieron reclamaciones que requieren una investigación más profunda.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t xml:space="preserve">Not Upheld Complaints: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>(Integer)  El soporte de la variable pertenece al conjunto {0,1,2,…,525}. El valor de cero significa que no hubieron reclamaciones no aceptadas por el Departamento de Servicios Financieros</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t xml:space="preserve">Total Complaints: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>(Integer) El soporte de la variable pertenece al conjunto {0,1,2,…,1350}. El valor de cero significa que no hubieron reclamaciones en total.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t xml:space="preserve">Premiums Written (in Millions): </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>(Float)  El soporte de la variable pertenece al intervalo [0.004, 2200). Es cercano a cero, por algunas razones: 
+* La compañía de seguros ha vendido pocas pólizas nuevas o ha perdido clientes en ese período.
+* La compañía de seguros ha cedido una gran parte de sus primas a las compañías de reaseguros para reducir su riesgo.
+* La compañía de seguros ha asumido poco o ningún reaseguro de otras compañías.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>Filing Year:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer) El soporte de la variable pertenece al conjunto {2009, 2016}, sin embargo para el desarrollo del análisis sólo se considerará el 2016. El valor de 0 no tiene sentido en esta variable.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>Rank:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF3C4043"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer) El soporte de la variable pertenece al conjunto {0,1,2,…,181}. En este conjunto de datos no hay aseguradoras cuyo valor sea 0 en esta variable, sin embargo, podría ser 0 si la empresa no ha recibido ninguna reclamación de sus clientes durante el período de tiempo considerado. Esto indicaría que la empresa tiene una alta calidad en sus productos o servicios, o que sus clientes están muy satisfechos con su atención. Sin embargo, también podría deberse a que la empresa tiene una baja participación en el mercado, o que sus clientes no tienen un canal adecuado para expresar sus reclamaciones.</t>
     </r>
   </si>
 </sst>
@@ -1387,7 +1523,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1502,6 +1638,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1548,28 +1722,40 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1930,7 +2116,7 @@
   <dimension ref="A1:K1359"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -49508,187 +49694,192 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD8C7D3-A9B9-4FAD-8C4D-ED91A348123F}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="B1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="118.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="118.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B1" s="4"/>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="2:3" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B2" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C2" s="6" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="2:3" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B3" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C3" s="5" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="31.5" customHeight="1">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="2:3" ht="31.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B4" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C4" s="5" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="29.25" thickTop="1">
+      <c r="B5" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" s="9"/>
+      <c r="C6" s="8" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" s="9"/>
+      <c r="C7" s="8" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" s="9"/>
+      <c r="C8" s="8" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" s="9"/>
+      <c r="C9" s="8" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10" s="9"/>
+      <c r="C10" s="8" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30">
-      <c r="A4" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="B4" s="7" t="s">
+    <row r="11" spans="2:3">
+      <c r="B11" s="9"/>
+      <c r="C11" s="8" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" s="9"/>
+      <c r="C12" s="8" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" s="9"/>
+      <c r="C13" s="8" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="5" t="s">
+    <row r="14" spans="2:3">
+      <c r="B14" s="9"/>
+      <c r="C14" s="8" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B15" s="10"/>
+      <c r="C15" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="144" thickTop="1">
+      <c r="B16" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="29.25">
+      <c r="B17" s="9"/>
+      <c r="C17" s="8" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="43.5">
+      <c r="B18" s="9"/>
+      <c r="C18" s="8" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="5" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="5" t="s">
+    <row r="19" spans="2:3" ht="29.25">
+      <c r="B19" s="9"/>
+      <c r="C19" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="29.25">
+      <c r="B20" s="9"/>
+      <c r="C20" s="8" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="29.25">
+      <c r="B21" s="9"/>
+      <c r="C21" s="8" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="29.25">
+      <c r="B22" s="9"/>
+      <c r="C22" s="8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="72">
+      <c r="B23" s="9"/>
+      <c r="C23" s="8" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="86.25">
+      <c r="B24" s="9"/>
+      <c r="C24" s="8" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="30" thickBot="1">
+      <c r="B25" s="10"/>
+      <c r="C25" s="5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B26" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="5" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="5" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="5" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="5" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="6"/>
-      <c r="B12" s="5" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="5" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="5" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="143.25">
-      <c r="A15" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="5" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="5" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="6"/>
-      <c r="B18" s="5" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="5" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="5" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="6"/>
-      <c r="B21" s="5" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="6"/>
-      <c r="B22" s="5" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="6"/>
-      <c r="B23" s="5" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="6"/>
-      <c r="B24" s="5" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>252</v>
-      </c>
-    </row>
+    <row r="27" spans="2:3" ht="15.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A4:A14"/>
-    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="B5:B15"/>
+    <mergeCell ref="B16:B25"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" display="https://www.kaggle.com/datasets/thedevastator/new-york-automobile-insurance-companies-complain" xr:uid="{8198716A-A829-4C93-862C-64A96F1EEBE5}"/>
+    <hyperlink ref="C2" r:id="rId1" display="https://www.kaggle.com/datasets/thedevastator/new-york-automobile-insurance-companies-complain" xr:uid="{8198716A-A829-4C93-862C-64A96F1EEBE5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>